<commit_message>
added new data dummy
</commit_message>
<xml_diff>
--- a/DataDummy.xlsx
+++ b/DataDummy.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aqsha\Kampus\POST\S3\Data Science\Tugas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoe\Documents\GitHub\pt-ifca-customer-segmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C98E788-43A8-4E00-80A9-4136CBE74F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
-  <si>
-    <t>Nama Customer</t>
-  </si>
-  <si>
-    <t>Pendapatan/Tahun</t>
-  </si>
-  <si>
-    <t>Bidang</t>
-  </si>
-  <si>
-    <t>Jumlah Karyawan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Urban Jakarta</t>
   </si>
@@ -96,12 +85,30 @@
   </si>
   <si>
     <t>Building Management</t>
+  </si>
+  <si>
+    <t>nama_customer</t>
+  </si>
+  <si>
+    <t>pendapatan_tahunan</t>
+  </si>
+  <si>
+    <t>bidang_perusahaan</t>
+  </si>
+  <si>
+    <t>jumlah_karyawan</t>
+  </si>
+  <si>
+    <t>usia_perusahaan</t>
+  </si>
+  <si>
+    <t>simbol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,271 +420,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="str">
+        <f>IF($D2="Developer","o",IF($D2="Mall","x","s"))</f>
+        <v>o</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B18" si="0">IF($D3="Developer","o",IF($D3="Mall","x","s"))</f>
+        <v>o</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>355</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>o</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1750</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>405</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>o</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3050</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>280</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>1200000000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>x</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>2100000000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>o</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>110</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>1750500000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>s</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5004</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>3050400000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>s</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3800</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>x</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2050</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>o</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3400</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>305</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>x</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>515</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>s</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1850</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
         <v>280</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4120600000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1100350000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>s</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>175</v>
+      </c>
+      <c r="F14">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>5004550000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3800200000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>o</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2455</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>x</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>265</v>
+      </c>
+      <c r="F16">
         <v>12</v>
       </c>
-      <c r="B10" s="1">
-        <v>2050200000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3400520000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4100750000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1">
-        <v>1850750000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>x</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7055</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>370</v>
+      </c>
+      <c r="F17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1">
-        <v>1500600000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2455500000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2150500000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>s</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3580</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1">
-        <v>7055150000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3580500000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18">
+      <c r="E18">
         <v>290</v>
+      </c>
+      <c r="F18">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>